<commit_message>
correccion en plantilla indicadores
</commit_message>
<xml_diff>
--- a/XLSX/plantillaIndicadores.xlsx
+++ b/XLSX/plantillaIndicadores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Residencia\ActualizacionDocente\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Final\actdoc\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B54793-FE7B-4877-96A2-1763ACBAD60E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01D7814-28B8-475C-A161-10926861635E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0C8322C2-4061-4828-B4CE-DCAA2CEACEC9}"/>
   </bookViews>
@@ -114,10 +114,10 @@
     <t>Totales</t>
   </si>
   <si>
-    <t>A continuación se muestran los indicadores totales por curso. (Nota: en caso de que un docente participe en más de un curso se consiera le considera como una persona  independiente en cada curso)</t>
-  </si>
-  <si>
     <t>Indicadores de Participantes Aprobados del Curso</t>
+  </si>
+  <si>
+    <t>A continuación se muestran los indicadores totales por curso. (Nota: en caso de que un docente participe en más de un curso se considera como una persona independiente en cada curso)</t>
   </si>
 </sst>
 </file>
@@ -434,6 +434,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -497,7 +498,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,7 +867,7 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,63 +892,63 @@
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="17"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="20"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="23"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="24"/>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G8" s="10"/>
@@ -957,71 +957,71 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
+      <c r="A9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="27" t="s">
+      <c r="D11" s="31"/>
+      <c r="E11" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="11" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11" t="s">
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11" t="s">
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11" t="s">
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="U11" s="11"/>
+      <c r="U11" s="12"/>
     </row>
     <row r="12" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
@@ -2127,6 +2127,11 @@
     <row r="81" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="Q11:S11"/>
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F3:L5"/>
@@ -2134,11 +2139,6 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="M11:P11"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="Q11:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>